<commit_message>
ajuste codigo e arquivo de dados
</commit_message>
<xml_diff>
--- a/dados/ListaCredenciamento.xlsx
+++ b/dados/ListaCredenciamento.xlsx
@@ -592,7 +592,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -704,7 +704,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1284,7 +1284,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -1551,6 +1551,16 @@
           <t>SIM</t>
         </is>
       </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>2023-10-26 23:22:19.022588</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1635,7 +1645,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -1752,7 +1762,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -1869,7 +1879,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -2006,7 +2016,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -2123,7 +2133,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
@@ -2250,7 +2260,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
@@ -2362,24 +2372,24 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>Não credenciado</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>Não credenciado</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
           <t>não</t>
         </is>
       </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>Não credenciado</t>
-        </is>
-      </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>Não credenciado</t>
-        </is>
-      </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>não</t>
-        </is>
-      </c>
       <c r="Z17" t="inlineStr">
         <is>
           <t>sim</t>
@@ -2393,6 +2403,16 @@
       <c r="AC17" t="inlineStr">
         <is>
           <t>SIM</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>2023-10-27 19:13:40.378144</t>
         </is>
       </c>
     </row>
@@ -2474,7 +2494,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
@@ -2586,7 +2606,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
@@ -2723,7 +2743,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
@@ -2835,7 +2855,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -2947,7 +2967,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
@@ -3064,7 +3084,7 @@
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
@@ -3206,7 +3226,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
@@ -3333,7 +3353,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
@@ -3435,7 +3455,7 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
@@ -3552,7 +3572,7 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
@@ -3679,7 +3699,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
@@ -3791,7 +3811,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
@@ -3913,7 +3933,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
@@ -4045,7 +4065,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W31" t="inlineStr">
@@ -4142,7 +4162,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
@@ -4259,7 +4279,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
@@ -4371,7 +4391,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W34" t="inlineStr">
@@ -4483,7 +4503,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W35" t="inlineStr">
@@ -4605,7 +4625,7 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W36" t="inlineStr">
@@ -4712,7 +4732,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W37" t="inlineStr">
@@ -4854,7 +4874,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W38" t="inlineStr">
@@ -4971,7 +4991,7 @@
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W39" t="inlineStr">
@@ -5093,7 +5113,7 @@
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W40" t="inlineStr">
@@ -5210,7 +5230,7 @@
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W41" t="inlineStr">
@@ -5327,7 +5347,7 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W42" t="inlineStr">
@@ -5439,7 +5459,7 @@
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W43" t="inlineStr">
@@ -5556,7 +5576,7 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W44" t="inlineStr">
@@ -5673,7 +5693,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W45" t="inlineStr">
@@ -5785,7 +5805,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W46" t="inlineStr">
@@ -5897,7 +5917,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W47" t="inlineStr">
@@ -6009,7 +6029,7 @@
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W48" t="inlineStr">
@@ -6136,7 +6156,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W49" t="inlineStr">
@@ -6248,7 +6268,7 @@
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W50" t="inlineStr">
@@ -6355,7 +6375,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W51" t="inlineStr">
@@ -6467,7 +6487,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W52" t="inlineStr">
@@ -6574,7 +6594,7 @@
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W53" t="inlineStr">
@@ -6691,7 +6711,7 @@
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W54" t="inlineStr">
@@ -6803,7 +6823,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W55" t="inlineStr">
@@ -6920,7 +6940,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W56" t="inlineStr">
@@ -7037,7 +7057,7 @@
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W57" t="inlineStr">
@@ -7149,7 +7169,7 @@
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W58" t="inlineStr">
@@ -7261,7 +7281,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W59" t="inlineStr">
@@ -7378,7 +7398,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W60" t="inlineStr">
@@ -7515,7 +7535,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W61" t="inlineStr">
@@ -7657,7 +7677,7 @@
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W62" t="inlineStr">
@@ -7769,7 +7789,7 @@
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W63" t="inlineStr">
@@ -7916,7 +7936,7 @@
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W64" t="inlineStr">
@@ -8028,7 +8048,7 @@
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W65" t="inlineStr">
@@ -8165,7 +8185,7 @@
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W66" t="inlineStr">
@@ -8277,7 +8297,7 @@
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W67" t="inlineStr">
@@ -8404,7 +8424,7 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W68" t="inlineStr">
@@ -8521,7 +8541,7 @@
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W69" t="inlineStr">
@@ -8638,7 +8658,7 @@
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W70" t="inlineStr">
@@ -8755,7 +8775,7 @@
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W71" t="inlineStr">
@@ -8897,7 +8917,7 @@
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W72" t="inlineStr">
@@ -9014,7 +9034,7 @@
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W73" t="inlineStr">
@@ -9126,7 +9146,7 @@
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W74" t="inlineStr">
@@ -9238,7 +9258,7 @@
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W75" t="inlineStr">
@@ -9360,7 +9380,7 @@
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W76" t="inlineStr">
@@ -9472,7 +9492,7 @@
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W77" t="inlineStr">
@@ -9584,7 +9604,7 @@
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W78" t="inlineStr">
@@ -9701,7 +9721,7 @@
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W79" t="inlineStr">
@@ -9813,7 +9833,7 @@
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W80" t="inlineStr">
@@ -9940,7 +9960,7 @@
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W81" t="inlineStr">
@@ -10052,7 +10072,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W82" t="inlineStr">
@@ -10169,7 +10189,7 @@
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W83" t="inlineStr">
@@ -10281,7 +10301,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W84" t="inlineStr">
@@ -10408,7 +10428,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W85" t="inlineStr">
@@ -10525,7 +10545,7 @@
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W86" t="inlineStr">
@@ -10637,7 +10657,7 @@
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W87" t="inlineStr">
@@ -10749,7 +10769,7 @@
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W88" t="inlineStr">
@@ -10861,7 +10881,7 @@
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W89" t="inlineStr">
@@ -10978,7 +10998,7 @@
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W90" t="inlineStr">
@@ -11095,7 +11115,7 @@
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W91" t="inlineStr">
@@ -11202,7 +11222,7 @@
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W92" t="inlineStr">
@@ -11309,7 +11329,7 @@
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W93" t="inlineStr">
@@ -11426,7 +11446,7 @@
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W94" t="inlineStr">
@@ -11558,7 +11578,7 @@
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W95" t="inlineStr">
@@ -11690,7 +11710,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W96" t="inlineStr">
@@ -11812,7 +11832,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W97" t="inlineStr">
@@ -11924,7 +11944,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W98" t="inlineStr">
@@ -12051,7 +12071,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W99" t="inlineStr">
@@ -12193,7 +12213,7 @@
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W100" t="inlineStr">
@@ -12325,7 +12345,7 @@
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W101" t="inlineStr">
@@ -12442,7 +12462,7 @@
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W102" t="inlineStr">
@@ -12559,7 +12579,7 @@
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W103" t="inlineStr">
@@ -12701,7 +12721,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W104" t="inlineStr">
@@ -12818,7 +12838,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W105" t="inlineStr">
@@ -12930,7 +12950,7 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W106" t="inlineStr">
@@ -13047,7 +13067,7 @@
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W107" t="inlineStr">
@@ -13164,7 +13184,7 @@
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W108" t="inlineStr">
@@ -13281,7 +13301,7 @@
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W109" t="inlineStr">
@@ -13393,7 +13413,7 @@
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W110" t="inlineStr">
@@ -13505,7 +13525,7 @@
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W111" t="inlineStr">
@@ -13632,7 +13652,7 @@
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W112" t="inlineStr">
@@ -13749,7 +13769,7 @@
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W113" t="inlineStr">
@@ -13866,7 +13886,7 @@
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W114" t="inlineStr">
@@ -13998,7 +14018,7 @@
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W115" t="inlineStr">
@@ -14110,7 +14130,7 @@
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W116" t="inlineStr">
@@ -14227,7 +14247,7 @@
       </c>
       <c r="V117" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W117" t="inlineStr">
@@ -14344,7 +14364,7 @@
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W118" t="inlineStr">
@@ -14446,7 +14466,7 @@
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W119" t="inlineStr">
@@ -14558,7 +14578,7 @@
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W120" t="inlineStr">
@@ -14680,7 +14700,7 @@
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W121" t="inlineStr">
@@ -14812,7 +14832,7 @@
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W122" t="inlineStr">
@@ -14929,7 +14949,7 @@
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W123" t="inlineStr">
@@ -15036,7 +15056,7 @@
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W124" t="inlineStr">
@@ -15148,7 +15168,7 @@
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W125" t="inlineStr">
@@ -15285,7 +15305,7 @@
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W126" t="inlineStr">
@@ -15402,7 +15422,7 @@
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W127" t="inlineStr">
@@ -15519,7 +15539,7 @@
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W128" t="inlineStr">
@@ -15636,7 +15656,7 @@
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W129" t="inlineStr">
@@ -15870,7 +15890,7 @@
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W131" t="inlineStr">
@@ -15987,7 +16007,7 @@
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W132" t="inlineStr">
@@ -16099,7 +16119,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W133" t="inlineStr">
@@ -16216,7 +16236,7 @@
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W134" t="inlineStr">
@@ -16338,7 +16358,7 @@
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W135" t="inlineStr">
@@ -16465,7 +16485,7 @@
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W136" t="inlineStr">
@@ -16577,7 +16597,7 @@
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W137" t="inlineStr">
@@ -16689,7 +16709,7 @@
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W138" t="inlineStr">
@@ -16831,7 +16851,7 @@
       </c>
       <c r="V139" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W139" t="inlineStr">
@@ -16943,7 +16963,7 @@
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W140" t="inlineStr">
@@ -17055,7 +17075,7 @@
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W141" t="inlineStr">
@@ -17172,7 +17192,7 @@
       </c>
       <c r="V142" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W142" t="inlineStr">
@@ -17284,7 +17304,7 @@
       </c>
       <c r="V143" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W143" t="inlineStr">
@@ -17396,7 +17416,7 @@
       </c>
       <c r="V144" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W144" t="inlineStr">
@@ -17508,7 +17528,7 @@
       </c>
       <c r="V145" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W145" t="inlineStr">
@@ -17625,7 +17645,7 @@
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W146" t="inlineStr">
@@ -17737,7 +17757,7 @@
       </c>
       <c r="V147" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W147" t="inlineStr">
@@ -17859,7 +17879,7 @@
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W148" t="inlineStr">
@@ -17971,7 +17991,7 @@
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W149" t="inlineStr">
@@ -18108,7 +18128,7 @@
       </c>
       <c r="V150" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W150" t="inlineStr">
@@ -18220,7 +18240,7 @@
       </c>
       <c r="V151" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W151" t="inlineStr">
@@ -18317,7 +18337,7 @@
       </c>
       <c r="V152" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W152" t="inlineStr">
@@ -18409,7 +18429,7 @@
       </c>
       <c r="V153" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W153" t="inlineStr">
@@ -18486,7 +18506,7 @@
       </c>
       <c r="V154" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W154" t="inlineStr">
@@ -18553,7 +18573,7 @@
       </c>
       <c r="V155" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W155" t="inlineStr">
@@ -18630,7 +18650,7 @@
       </c>
       <c r="V156" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W156" t="inlineStr">
@@ -18732,7 +18752,7 @@
       </c>
       <c r="V157" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W157" t="inlineStr">
@@ -18834,7 +18854,7 @@
       </c>
       <c r="V158" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W158" t="inlineStr">
@@ -18926,7 +18946,7 @@
       </c>
       <c r="V159" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W159" t="inlineStr">
@@ -19023,7 +19043,7 @@
       </c>
       <c r="V160" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W160" t="inlineStr">
@@ -19140,7 +19160,7 @@
       </c>
       <c r="V161" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W161" t="inlineStr">
@@ -19257,7 +19277,7 @@
       </c>
       <c r="V162" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W162" t="inlineStr">
@@ -19369,7 +19389,7 @@
       </c>
       <c r="V163" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W163" t="inlineStr">
@@ -19481,7 +19501,7 @@
       </c>
       <c r="V164" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W164" t="inlineStr">
@@ -19588,7 +19608,7 @@
       </c>
       <c r="V165" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W165" t="inlineStr">
@@ -19695,7 +19715,7 @@
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W166" t="inlineStr">
@@ -19812,7 +19832,7 @@
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W167" t="inlineStr">
@@ -19924,7 +19944,7 @@
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W168" t="inlineStr">
@@ -20041,7 +20061,7 @@
       </c>
       <c r="V169" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W169" t="inlineStr">
@@ -20168,7 +20188,7 @@
       </c>
       <c r="V170" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W170" t="inlineStr">
@@ -20285,7 +20305,7 @@
       </c>
       <c r="V171" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W171" t="inlineStr">
@@ -20402,7 +20422,7 @@
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W172" t="inlineStr">
@@ -20509,7 +20529,7 @@
       </c>
       <c r="V173" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W173" t="inlineStr">
@@ -20626,7 +20646,7 @@
       </c>
       <c r="V174" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W174" t="inlineStr">
@@ -20753,7 +20773,7 @@
       </c>
       <c r="V175" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W175" t="inlineStr">
@@ -20860,7 +20880,7 @@
       </c>
       <c r="V176" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W176" t="inlineStr">
@@ -20962,7 +20982,7 @@
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W177" t="inlineStr">
@@ -21074,7 +21094,7 @@
       </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W178" t="inlineStr">
@@ -21206,7 +21226,7 @@
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W179" t="inlineStr">
@@ -21343,7 +21363,7 @@
       </c>
       <c r="V180" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W180" t="inlineStr">
@@ -21460,7 +21480,7 @@
       </c>
       <c r="V181" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W181" t="inlineStr">
@@ -21577,7 +21597,7 @@
       </c>
       <c r="V182" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W182" t="inlineStr">
@@ -21699,7 +21719,7 @@
       </c>
       <c r="V183" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W183" t="inlineStr">
@@ -21816,7 +21836,7 @@
       </c>
       <c r="V184" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W184" t="inlineStr">
@@ -21928,7 +21948,7 @@
       </c>
       <c r="V185" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W185" t="inlineStr">
@@ -22045,7 +22065,7 @@
       </c>
       <c r="V186" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W186" t="inlineStr">
@@ -22152,7 +22172,7 @@
       </c>
       <c r="V187" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W187" t="inlineStr">
@@ -22274,7 +22294,7 @@
       </c>
       <c r="V188" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W188" t="inlineStr">
@@ -22431,7 +22451,7 @@
       </c>
       <c r="V189" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W189" t="inlineStr">
@@ -22548,7 +22568,7 @@
       </c>
       <c r="V190" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W190" t="inlineStr">
@@ -22670,7 +22690,7 @@
       </c>
       <c r="V191" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W191" t="inlineStr">
@@ -22782,7 +22802,7 @@
       </c>
       <c r="V192" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W192" t="inlineStr">
@@ -22899,7 +22919,7 @@
       </c>
       <c r="V193" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W193" t="inlineStr">
@@ -23016,7 +23036,7 @@
       </c>
       <c r="V194" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W194" t="inlineStr">
@@ -23128,7 +23148,7 @@
       </c>
       <c r="V195" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W195" t="inlineStr">
@@ -23245,7 +23265,7 @@
       </c>
       <c r="V196" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W196" t="inlineStr">
@@ -23362,7 +23382,7 @@
       </c>
       <c r="V197" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W197" t="inlineStr">
@@ -23489,7 +23509,7 @@
       </c>
       <c r="V198" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W198" t="inlineStr">
@@ -23606,7 +23626,7 @@
       </c>
       <c r="V199" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W199" t="inlineStr">
@@ -23723,7 +23743,7 @@
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W200" t="inlineStr">
@@ -23835,7 +23855,7 @@
       </c>
       <c r="V201" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W201" t="inlineStr">
@@ -23952,7 +23972,7 @@
       </c>
       <c r="V202" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W202" t="inlineStr">
@@ -24059,7 +24079,7 @@
       </c>
       <c r="V203" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W203" t="inlineStr">
@@ -24171,7 +24191,7 @@
       </c>
       <c r="V204" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W204" t="inlineStr">
@@ -24283,7 +24303,7 @@
       </c>
       <c r="V205" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W205" t="inlineStr">
@@ -24395,7 +24415,7 @@
       </c>
       <c r="V206" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W206" t="inlineStr">
@@ -24507,7 +24527,7 @@
       </c>
       <c r="V207" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W207" t="inlineStr">
@@ -24619,7 +24639,7 @@
       </c>
       <c r="V208" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W208" t="inlineStr">
@@ -24731,7 +24751,7 @@
       </c>
       <c r="V209" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W209" t="inlineStr">
@@ -24843,7 +24863,7 @@
       </c>
       <c r="V210" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W210" t="inlineStr">
@@ -24955,7 +24975,7 @@
       </c>
       <c r="V211" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W211" t="inlineStr">
@@ -25072,7 +25092,7 @@
       </c>
       <c r="V212" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W212" t="inlineStr">
@@ -25184,7 +25204,7 @@
       </c>
       <c r="V213" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W213" t="inlineStr">
@@ -25296,7 +25316,7 @@
       </c>
       <c r="V214" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W214" t="inlineStr">
@@ -25413,7 +25433,7 @@
       </c>
       <c r="V215" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W215" t="inlineStr">
@@ -25530,7 +25550,7 @@
       </c>
       <c r="V216" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W216" t="inlineStr">
@@ -25647,7 +25667,7 @@
       </c>
       <c r="V217" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W217" t="inlineStr">
@@ -25764,7 +25784,7 @@
       </c>
       <c r="V218" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W218" t="inlineStr">
@@ -25871,7 +25891,7 @@
       </c>
       <c r="V219" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W219" t="inlineStr">
@@ -25973,7 +25993,7 @@
       </c>
       <c r="V220" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W220" t="inlineStr">
@@ -26100,7 +26120,7 @@
       </c>
       <c r="V221" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W221" t="inlineStr">
@@ -26222,7 +26242,7 @@
       </c>
       <c r="V222" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W222" t="inlineStr">
@@ -26359,7 +26379,7 @@
       </c>
       <c r="V223" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W223" t="inlineStr">
@@ -26476,7 +26496,7 @@
       </c>
       <c r="V224" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W224" t="inlineStr">
@@ -26583,7 +26603,7 @@
       </c>
       <c r="V225" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W225" t="inlineStr">
@@ -26730,7 +26750,7 @@
       </c>
       <c r="V226" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W226" t="inlineStr">
@@ -26847,7 +26867,7 @@
       </c>
       <c r="V227" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W227" t="inlineStr">
@@ -26959,7 +26979,7 @@
       </c>
       <c r="V228" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W228" t="inlineStr">
@@ -27101,7 +27121,7 @@
       </c>
       <c r="V229" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W229" t="inlineStr">
@@ -27238,7 +27258,7 @@
       </c>
       <c r="V230" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W230" t="inlineStr">
@@ -27335,7 +27355,7 @@
       </c>
       <c r="V231" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W231" t="inlineStr">
@@ -27452,7 +27472,7 @@
       </c>
       <c r="V232" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W232" t="inlineStr">
@@ -27569,7 +27589,7 @@
       </c>
       <c r="V233" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W233" t="inlineStr">
@@ -27686,7 +27706,7 @@
       </c>
       <c r="V234" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W234" t="inlineStr">
@@ -27803,7 +27823,7 @@
       </c>
       <c r="V235" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W235" t="inlineStr">
@@ -27930,7 +27950,7 @@
       </c>
       <c r="V236" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W236" t="inlineStr">
@@ -28057,7 +28077,7 @@
       </c>
       <c r="V237" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W237" t="inlineStr">
@@ -28169,7 +28189,7 @@
       </c>
       <c r="V238" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W238" t="inlineStr">
@@ -28281,7 +28301,7 @@
       </c>
       <c r="V239" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W239" t="inlineStr">
@@ -28398,7 +28418,7 @@
       </c>
       <c r="V240" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W240" t="inlineStr">
@@ -28515,7 +28535,7 @@
       </c>
       <c r="V241" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W241" t="inlineStr">
@@ -28627,7 +28647,7 @@
       </c>
       <c r="V242" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W242" t="inlineStr">
@@ -28739,7 +28759,7 @@
       </c>
       <c r="V243" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W243" t="inlineStr">
@@ -28851,7 +28871,7 @@
       </c>
       <c r="V244" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W244" t="inlineStr">
@@ -28953,7 +28973,7 @@
       </c>
       <c r="V245" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W245" t="inlineStr">
@@ -29070,7 +29090,7 @@
       </c>
       <c r="V246" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W246" t="inlineStr">
@@ -29167,7 +29187,7 @@
       </c>
       <c r="V247" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W247" t="inlineStr">
@@ -29264,7 +29284,7 @@
       </c>
       <c r="V248" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W248" t="inlineStr">
@@ -29381,7 +29401,7 @@
       </c>
       <c r="V249" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W249" t="inlineStr">
@@ -29498,7 +29518,7 @@
       </c>
       <c r="V250" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W250" t="inlineStr">
@@ -29615,7 +29635,7 @@
       </c>
       <c r="V251" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W251" t="inlineStr">
@@ -29732,7 +29752,7 @@
       </c>
       <c r="V252" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W252" t="inlineStr">
@@ -29849,7 +29869,7 @@
       </c>
       <c r="V253" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W253" t="inlineStr">
@@ -29971,7 +29991,7 @@
       </c>
       <c r="V254" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W254" t="inlineStr">
@@ -30088,7 +30108,7 @@
       </c>
       <c r="V255" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W255" t="inlineStr">
@@ -30200,7 +30220,7 @@
       </c>
       <c r="V256" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W256" t="inlineStr">
@@ -30312,7 +30332,7 @@
       </c>
       <c r="V257" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W257" t="inlineStr">
@@ -30439,7 +30459,7 @@
       </c>
       <c r="V258" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W258" t="inlineStr">
@@ -30556,7 +30576,7 @@
       </c>
       <c r="V259" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W259" t="inlineStr">
@@ -30673,7 +30693,7 @@
       </c>
       <c r="V260" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W260" t="inlineStr">
@@ -30790,7 +30810,7 @@
       </c>
       <c r="V261" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W261" t="inlineStr">
@@ -30907,7 +30927,7 @@
       </c>
       <c r="V262" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W262" t="inlineStr">
@@ -31024,7 +31044,7 @@
       </c>
       <c r="V263" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W263" t="inlineStr">
@@ -31136,7 +31156,7 @@
       </c>
       <c r="V264" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W264" t="inlineStr">
@@ -31253,7 +31273,7 @@
       </c>
       <c r="V265" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W265" t="inlineStr">
@@ -31365,7 +31385,7 @@
       </c>
       <c r="V266" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W266" t="inlineStr">
@@ -31477,7 +31497,7 @@
       </c>
       <c r="V267" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W267" t="inlineStr">
@@ -31594,7 +31614,7 @@
       </c>
       <c r="V268" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W268" t="inlineStr">
@@ -31711,7 +31731,7 @@
       </c>
       <c r="V269" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W269" t="inlineStr">
@@ -31828,7 +31848,7 @@
       </c>
       <c r="V270" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W270" t="inlineStr">
@@ -31945,7 +31965,7 @@
       </c>
       <c r="V271" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W271" t="inlineStr">
@@ -32062,7 +32082,7 @@
       </c>
       <c r="V272" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W272" t="inlineStr">
@@ -32169,7 +32189,7 @@
       </c>
       <c r="V273" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W273" t="inlineStr">
@@ -32286,7 +32306,7 @@
       </c>
       <c r="V274" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W274" t="inlineStr">
@@ -32403,7 +32423,7 @@
       </c>
       <c r="V275" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W275" t="inlineStr">
@@ -32520,7 +32540,7 @@
       </c>
       <c r="V276" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W276" t="inlineStr">
@@ -32637,7 +32657,7 @@
       </c>
       <c r="V277" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W277" t="inlineStr">
@@ -32749,7 +32769,7 @@
       </c>
       <c r="V278" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W278" t="inlineStr">
@@ -32871,7 +32891,7 @@
       </c>
       <c r="V279" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W279" t="inlineStr">
@@ -32983,7 +33003,7 @@
       </c>
       <c r="V280" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W280" t="inlineStr">
@@ -33100,7 +33120,7 @@
       </c>
       <c r="V281" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W281" t="inlineStr">
@@ -33217,7 +33237,7 @@
       </c>
       <c r="V282" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W282" t="inlineStr">
@@ -33334,7 +33354,7 @@
       </c>
       <c r="V283" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W283" t="inlineStr">
@@ -33451,7 +33471,7 @@
       </c>
       <c r="V284" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W284" t="inlineStr">
@@ -33568,7 +33588,7 @@
       </c>
       <c r="V285" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W285" t="inlineStr">
@@ -33695,7 +33715,7 @@
       </c>
       <c r="V286" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W286" t="inlineStr">
@@ -33812,7 +33832,7 @@
       </c>
       <c r="V287" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W287" t="inlineStr">
@@ -33929,7 +33949,7 @@
       </c>
       <c r="V288" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W288" t="inlineStr">
@@ -34041,7 +34061,7 @@
       </c>
       <c r="V289" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W289" t="inlineStr">
@@ -34153,7 +34173,7 @@
       </c>
       <c r="V290" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W290" t="inlineStr">
@@ -34270,7 +34290,7 @@
       </c>
       <c r="V291" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W291" t="inlineStr">
@@ -34382,7 +34402,7 @@
       </c>
       <c r="V292" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W292" t="inlineStr">
@@ -34499,7 +34519,7 @@
       </c>
       <c r="V293" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W293" t="inlineStr">
@@ -34616,7 +34636,7 @@
       </c>
       <c r="V294" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W294" t="inlineStr">
@@ -34733,7 +34753,7 @@
       </c>
       <c r="V295" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W295" t="inlineStr">
@@ -34850,7 +34870,7 @@
       </c>
       <c r="V296" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W296" t="inlineStr">
@@ -34962,7 +34982,7 @@
       </c>
       <c r="V297" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W297" t="inlineStr">
@@ -35074,7 +35094,7 @@
       </c>
       <c r="V298" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W298" t="inlineStr">
@@ -35191,7 +35211,7 @@
       </c>
       <c r="V299" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W299" t="inlineStr">
@@ -35308,7 +35328,7 @@
       </c>
       <c r="V300" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W300" t="inlineStr">
@@ -35425,7 +35445,7 @@
       </c>
       <c r="V301" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W301" t="inlineStr">
@@ -35532,7 +35552,7 @@
       </c>
       <c r="V302" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W302" t="inlineStr">
@@ -35644,7 +35664,7 @@
       </c>
       <c r="V303" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W303" t="inlineStr">
@@ -35766,7 +35786,7 @@
       </c>
       <c r="V304" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W304" t="inlineStr">
@@ -35908,7 +35928,7 @@
       </c>
       <c r="V305" t="inlineStr">
         <is>
-          <t>não</t>
+          <t>sim</t>
         </is>
       </c>
       <c r="W305" t="inlineStr">

</xml_diff>